<commit_message>
Actualización escalas de sugerencias
</commit_message>
<xml_diff>
--- a/Ligas/Liga_bolivia_2025.xlsx
+++ b/Ligas/Liga_bolivia_2025.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\raque\Desktop\ligas_datas\rockongo_web\Ligas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A4F42AD-CC1A-4CE9-B728-DE7400CC83F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48404140-E6B9-4FB2-BD04-E31E62413E54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="332" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="422" uniqueCount="81">
   <si>
     <t>Fecha</t>
   </si>
@@ -76,6 +76,9 @@
     <t>Posesión Visita (%)</t>
   </si>
   <si>
+    <t>Resultado</t>
+  </si>
+  <si>
     <t>2025-03-28</t>
   </si>
   <si>
@@ -85,12 +88,18 @@
     <t>Guabirá</t>
   </si>
   <si>
+    <t>L</t>
+  </si>
+  <si>
     <t>Nacional Potosí</t>
   </si>
   <si>
     <t>Always Ready</t>
   </si>
   <si>
+    <t>V</t>
+  </si>
+  <si>
     <t>2025-03-29</t>
   </si>
   <si>
@@ -136,6 +145,9 @@
     <t>2025-04-04</t>
   </si>
   <si>
+    <t>E</t>
+  </si>
+  <si>
     <t>2025-04-05</t>
   </si>
   <si>
@@ -247,16 +259,7 @@
     <t>2025-07-05</t>
   </si>
   <si>
-    <t>43%</t>
-  </si>
-  <si>
-    <t>57%</t>
-  </si>
-  <si>
     <t>2025-07-06</t>
-  </si>
-  <si>
-    <t>0%</t>
   </si>
   <si>
     <t>2025-07-07</t>
@@ -315,11 +318,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -622,33 +626,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:R101"/>
+  <dimension ref="A1:S102"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C85" workbookViewId="0">
-      <selection activeCell="P107" sqref="P107"/>
+    <sheetView tabSelected="1" topLeftCell="B79" workbookViewId="0">
+      <selection activeCell="C104" sqref="C104"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="10.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="20.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.5546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.21875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.44140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.44140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.33203125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="10.5546875" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="12.77734375" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="13" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="12.77734375" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="13" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="16.5546875" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="16.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -703,16 +697,19 @@
       <c r="R1" s="1" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S1" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D2">
         <v>4</v>
@@ -759,16 +756,19 @@
       <c r="R2">
         <v>47</v>
       </c>
-    </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B3" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C3" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D3">
         <v>0</v>
@@ -815,16 +815,19 @@
       <c r="R3">
         <v>54</v>
       </c>
-    </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="B4" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="C4" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="D4">
         <v>3</v>
@@ -871,16 +874,19 @@
       <c r="R4">
         <v>35</v>
       </c>
-    </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="B5" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="C5" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="D5">
         <v>2</v>
@@ -927,16 +933,19 @@
       <c r="R5">
         <v>56</v>
       </c>
-    </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="B6" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="C6" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="D6">
         <v>0</v>
@@ -983,16 +992,19 @@
       <c r="R6">
         <v>42</v>
       </c>
-    </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S6" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="B7" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="C7" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="D7">
         <v>3</v>
@@ -1039,16 +1051,19 @@
       <c r="R7">
         <v>48</v>
       </c>
-    </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S7" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="B8" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="C8" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="D8">
         <v>5</v>
@@ -1095,16 +1110,19 @@
       <c r="R8">
         <v>54</v>
       </c>
-    </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S8" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="B9" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="C9" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="D9">
         <v>3</v>
@@ -1151,16 +1169,19 @@
       <c r="R9">
         <v>39</v>
       </c>
-    </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S9" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
+        <v>40</v>
+      </c>
+      <c r="B10" t="s">
         <v>37</v>
       </c>
-      <c r="B10" t="s">
-        <v>34</v>
-      </c>
       <c r="C10" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D10">
         <v>0</v>
@@ -1207,16 +1228,19 @@
       <c r="R10">
         <v>51</v>
       </c>
-    </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S10" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="B11" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="C11" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="D11">
         <v>0</v>
@@ -1263,16 +1287,19 @@
       <c r="R11">
         <v>35</v>
       </c>
-    </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S11" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="B12" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C12" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="D12">
         <v>5</v>
@@ -1319,16 +1346,19 @@
       <c r="R12">
         <v>47</v>
       </c>
-    </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S12" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="B13" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="C13" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="D13">
         <v>2</v>
@@ -1375,16 +1405,19 @@
       <c r="R13">
         <v>52</v>
       </c>
-    </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S13" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
+        <v>42</v>
+      </c>
+      <c r="B14" t="s">
+        <v>24</v>
+      </c>
+      <c r="C14" t="s">
         <v>38</v>
-      </c>
-      <c r="B14" t="s">
-        <v>22</v>
-      </c>
-      <c r="C14" t="s">
-        <v>35</v>
       </c>
       <c r="D14">
         <v>2</v>
@@ -1431,16 +1464,19 @@
       <c r="R14">
         <v>30</v>
       </c>
-    </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S14" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="B15" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="C15" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="D15">
         <v>2</v>
@@ -1487,16 +1523,19 @@
       <c r="R15">
         <v>80</v>
       </c>
-    </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S15" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="B16" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="C16" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="D16">
         <v>0</v>
@@ -1543,16 +1582,19 @@
       <c r="R16">
         <v>45</v>
       </c>
-    </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S16" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="17" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
+        <v>43</v>
+      </c>
+      <c r="B17" t="s">
         <v>39</v>
       </c>
-      <c r="B17" t="s">
-        <v>36</v>
-      </c>
       <c r="C17" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="D17">
         <v>2</v>
@@ -1599,16 +1641,19 @@
       <c r="R17">
         <v>48</v>
       </c>
-    </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S17" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="18" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="B18" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="C18" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="D18">
         <v>0</v>
@@ -1655,16 +1700,19 @@
       <c r="R18">
         <v>39</v>
       </c>
-    </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S18" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="19" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="B19" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="C19" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="D19">
         <v>0</v>
@@ -1711,16 +1759,19 @@
       <c r="R19">
         <v>42</v>
       </c>
-    </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S19" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="20" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="B20" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C20" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="D20">
         <v>1</v>
@@ -1767,16 +1818,19 @@
       <c r="R20">
         <v>50</v>
       </c>
-    </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S20" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="21" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="B21" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="C21" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="D21">
         <v>5</v>
@@ -1823,16 +1877,19 @@
       <c r="R21">
         <v>37</v>
       </c>
-    </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S21" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="22" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="B22" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="C22" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="D22">
         <v>2</v>
@@ -1879,16 +1936,19 @@
       <c r="R22">
         <v>51</v>
       </c>
-    </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S22" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="23" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="B23" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="C23" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="D23">
         <v>0</v>
@@ -1935,16 +1995,19 @@
       <c r="R23">
         <v>43</v>
       </c>
-    </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S23" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="24" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="B24" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="C24" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D24">
         <v>1</v>
@@ -1991,16 +2054,19 @@
       <c r="R24">
         <v>44</v>
       </c>
-    </row>
-    <row r="25" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S24" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="25" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="B25" t="s">
+        <v>23</v>
+      </c>
+      <c r="C25" t="s">
         <v>21</v>
-      </c>
-      <c r="C25" t="s">
-        <v>20</v>
       </c>
       <c r="D25">
         <v>3</v>
@@ -2047,16 +2113,19 @@
       <c r="R25">
         <v>35</v>
       </c>
-    </row>
-    <row r="26" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S25" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="26" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="B26" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="C26" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="D26">
         <v>2</v>
@@ -2103,16 +2172,19 @@
       <c r="R26">
         <v>42</v>
       </c>
-    </row>
-    <row r="27" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S26" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="27" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="B27" t="s">
+        <v>39</v>
+      </c>
+      <c r="C27" t="s">
         <v>36</v>
-      </c>
-      <c r="C27" t="s">
-        <v>33</v>
       </c>
       <c r="D27">
         <v>3</v>
@@ -2159,16 +2231,19 @@
       <c r="R27">
         <v>38</v>
       </c>
-    </row>
-    <row r="28" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S27" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="28" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="B28" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="C28" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D28">
         <v>1</v>
@@ -2215,16 +2290,19 @@
       <c r="R28">
         <v>58</v>
       </c>
-    </row>
-    <row r="29" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S28" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="29" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="B29" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C29" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="D29">
         <v>2</v>
@@ -2271,16 +2349,19 @@
       <c r="R29">
         <v>39</v>
       </c>
-    </row>
-    <row r="30" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S29" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="30" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="B30" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="C30" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="D30">
         <v>3</v>
@@ -2327,16 +2408,19 @@
       <c r="R30">
         <v>32</v>
       </c>
-    </row>
-    <row r="31" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S30" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="31" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="B31" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C31" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="D31">
         <v>2</v>
@@ -2383,16 +2467,19 @@
       <c r="R31">
         <v>69</v>
       </c>
-    </row>
-    <row r="32" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S31" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="32" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="B32" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="C32" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="D32">
         <v>1</v>
@@ -2439,16 +2526,19 @@
       <c r="R32">
         <v>40</v>
       </c>
-    </row>
-    <row r="33" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S32" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="33" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="B33" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="C33" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="D33">
         <v>0</v>
@@ -2495,16 +2585,19 @@
       <c r="R33">
         <v>39</v>
       </c>
-    </row>
-    <row r="34" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S33" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="34" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="B34" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="C34" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="D34">
         <v>2</v>
@@ -2551,16 +2644,19 @@
       <c r="R34">
         <v>34</v>
       </c>
-    </row>
-    <row r="35" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S34" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="35" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="B35" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C35" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="D35">
         <v>1</v>
@@ -2607,16 +2703,19 @@
       <c r="R35">
         <v>53</v>
       </c>
-    </row>
-    <row r="36" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S35" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="36" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="B36" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="C36" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="D36">
         <v>1</v>
@@ -2663,16 +2762,19 @@
       <c r="R36">
         <v>48</v>
       </c>
-    </row>
-    <row r="37" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S36" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="37" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="B37" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="C37" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="D37">
         <v>1</v>
@@ -2719,16 +2821,19 @@
       <c r="R37">
         <v>44</v>
       </c>
-    </row>
-    <row r="38" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S37" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="38" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="B38" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="C38" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="D38">
         <v>1</v>
@@ -2775,16 +2880,19 @@
       <c r="R38">
         <v>54</v>
       </c>
-    </row>
-    <row r="39" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S38" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="39" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="B39" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C39" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="D39">
         <v>1</v>
@@ -2831,16 +2939,19 @@
       <c r="R39">
         <v>52</v>
       </c>
-    </row>
-    <row r="40" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S39" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="40" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="B40" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C40" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D40">
         <v>0</v>
@@ -2887,16 +2998,19 @@
       <c r="R40">
         <v>53</v>
       </c>
-    </row>
-    <row r="41" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S40" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="41" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="B41" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="C41" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="D41">
         <v>5</v>
@@ -2943,16 +3057,19 @@
       <c r="R41">
         <v>31</v>
       </c>
-    </row>
-    <row r="42" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S41" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="42" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="B42" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="C42" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="D42">
         <v>4</v>
@@ -2999,16 +3116,19 @@
       <c r="R42">
         <v>53</v>
       </c>
-    </row>
-    <row r="43" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S42" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="43" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="B43" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="C43" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D43">
         <v>5</v>
@@ -3055,16 +3175,19 @@
       <c r="R43">
         <v>41</v>
       </c>
-    </row>
-    <row r="44" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S43" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="44" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="B44" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="C44" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="D44">
         <v>0</v>
@@ -3111,16 +3234,19 @@
       <c r="R44">
         <v>45</v>
       </c>
-    </row>
-    <row r="45" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S44" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="45" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="B45" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="C45" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="D45">
         <v>0</v>
@@ -3167,16 +3293,19 @@
       <c r="R45">
         <v>67</v>
       </c>
-    </row>
-    <row r="46" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S45" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="46" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="B46" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="C46" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D46">
         <v>2</v>
@@ -3223,16 +3352,19 @@
       <c r="R46">
         <v>46</v>
       </c>
-    </row>
-    <row r="47" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S46" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="47" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="B47" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="C47" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="D47">
         <v>5</v>
@@ -3279,16 +3411,19 @@
       <c r="R47">
         <v>33</v>
       </c>
-    </row>
-    <row r="48" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S47" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="48" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="B48" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="C48" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D48">
         <v>2</v>
@@ -3335,16 +3470,19 @@
       <c r="R48">
         <v>54</v>
       </c>
-    </row>
-    <row r="49" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S48" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="49" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="B49" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="C49" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="D49">
         <v>3</v>
@@ -3391,16 +3529,19 @@
       <c r="R49">
         <v>41</v>
       </c>
-    </row>
-    <row r="50" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S49" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="50" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="B50" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C50" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="D50">
         <v>2</v>
@@ -3447,16 +3588,19 @@
       <c r="R50">
         <v>46</v>
       </c>
-    </row>
-    <row r="51" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S50" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="51" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="B51" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C51" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="D51">
         <v>3</v>
@@ -3503,16 +3647,19 @@
       <c r="R51">
         <v>42</v>
       </c>
-    </row>
-    <row r="52" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S51" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="52" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="B52" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="C52" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="D52">
         <v>5</v>
@@ -3559,16 +3706,19 @@
       <c r="R52">
         <v>69</v>
       </c>
-    </row>
-    <row r="53" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S52" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="53" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="B53" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C53" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="D53">
         <v>1</v>
@@ -3615,16 +3765,19 @@
       <c r="R53">
         <v>34</v>
       </c>
-    </row>
-    <row r="54" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S53" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="54" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="B54" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="C54" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="D54">
         <v>6</v>
@@ -3671,16 +3824,19 @@
       <c r="R54">
         <v>53</v>
       </c>
-    </row>
-    <row r="55" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S54" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="55" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="B55" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="C55" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="D55">
         <v>0</v>
@@ -3727,16 +3883,19 @@
       <c r="R55">
         <v>66</v>
       </c>
-    </row>
-    <row r="56" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S55" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="56" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="B56" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="C56" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D56">
         <v>1</v>
@@ -3783,16 +3942,19 @@
       <c r="R56">
         <v>31</v>
       </c>
-    </row>
-    <row r="57" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S56" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="57" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="B57" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C57" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="D57">
         <v>3</v>
@@ -3839,16 +4001,19 @@
       <c r="R57">
         <v>43</v>
       </c>
-    </row>
-    <row r="58" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S57" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="58" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="B58" t="s">
+        <v>35</v>
+      </c>
+      <c r="C58" t="s">
         <v>32</v>
-      </c>
-      <c r="C58" t="s">
-        <v>29</v>
       </c>
       <c r="D58">
         <v>3</v>
@@ -3895,16 +4060,19 @@
       <c r="R58">
         <v>43</v>
       </c>
-    </row>
-    <row r="59" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S58" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="59" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="B59" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="C59" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D59">
         <v>2</v>
@@ -3951,16 +4119,19 @@
       <c r="R59">
         <v>58</v>
       </c>
-    </row>
-    <row r="60" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S59" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="60" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="B60" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="C60" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D60">
         <v>0</v>
@@ -4007,16 +4178,19 @@
       <c r="R60">
         <v>39</v>
       </c>
-    </row>
-    <row r="61" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S60" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="61" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="B61" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="C61" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="D61">
         <v>2</v>
@@ -4063,16 +4237,19 @@
       <c r="R61">
         <v>53</v>
       </c>
-    </row>
-    <row r="62" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S61" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="62" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="B62" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="C62" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="D62">
         <v>3</v>
@@ -4119,16 +4296,19 @@
       <c r="R62">
         <v>49</v>
       </c>
-    </row>
-    <row r="63" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S62" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="63" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="B63" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C63" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="D63">
         <v>1</v>
@@ -4175,16 +4355,19 @@
       <c r="R63">
         <v>69</v>
       </c>
-    </row>
-    <row r="64" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S63" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="64" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="B64" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="C64" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="D64">
         <v>0</v>
@@ -4231,16 +4414,19 @@
       <c r="R64">
         <v>37</v>
       </c>
-    </row>
-    <row r="65" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S64" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="65" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="B65" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C65" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="D65">
         <v>5</v>
@@ -4287,16 +4473,19 @@
       <c r="R65">
         <v>35</v>
       </c>
-    </row>
-    <row r="66" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S65" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="66" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="B66" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="C66" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="D66">
         <v>0</v>
@@ -4343,16 +4532,19 @@
       <c r="R66">
         <v>61</v>
       </c>
-    </row>
-    <row r="67" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S66" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="67" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="B67" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C67" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="D67">
         <v>1</v>
@@ -4399,16 +4591,19 @@
       <c r="R67">
         <v>40</v>
       </c>
-    </row>
-    <row r="68" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S67" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="68" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="B68" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="C68" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="D68">
         <v>3</v>
@@ -4455,16 +4650,19 @@
       <c r="R68">
         <v>48</v>
       </c>
-    </row>
-    <row r="69" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S68" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="69" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="B69" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="C69" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="D69">
         <v>2</v>
@@ -4511,16 +4709,19 @@
       <c r="R69">
         <v>35</v>
       </c>
-    </row>
-    <row r="70" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S69" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="70" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="B70" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="C70" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="D70">
         <v>0</v>
@@ -4567,16 +4768,19 @@
       <c r="R70">
         <v>39</v>
       </c>
-    </row>
-    <row r="71" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S70" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="71" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="B71" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="C71" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="D71">
         <v>1</v>
@@ -4623,16 +4827,19 @@
       <c r="R71">
         <v>51</v>
       </c>
-    </row>
-    <row r="72" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S71" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="72" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="B72" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="C72" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="D72">
         <v>1</v>
@@ -4679,16 +4886,19 @@
       <c r="R72">
         <v>21</v>
       </c>
-    </row>
-    <row r="73" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S72" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="73" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="B73" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="C73" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D73">
         <v>1</v>
@@ -4735,16 +4945,19 @@
       <c r="R73">
         <v>33</v>
       </c>
-    </row>
-    <row r="74" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S73" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="74" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="B74" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="C74" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="D74">
         <v>1</v>
@@ -4791,16 +5004,19 @@
       <c r="R74">
         <v>51</v>
       </c>
-    </row>
-    <row r="75" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S74" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="75" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="B75" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="C75" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="D75">
         <v>2</v>
@@ -4847,16 +5063,19 @@
       <c r="R75">
         <v>60</v>
       </c>
-    </row>
-    <row r="76" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S75" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="76" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="B76" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="C76" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="D76">
         <v>3</v>
@@ -4903,16 +5122,19 @@
       <c r="R76">
         <v>43</v>
       </c>
-    </row>
-    <row r="77" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S76" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="77" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="B77" t="s">
+        <v>27</v>
+      </c>
+      <c r="C77" t="s">
         <v>24</v>
-      </c>
-      <c r="C77" t="s">
-        <v>22</v>
       </c>
       <c r="D77">
         <v>2</v>
@@ -4959,16 +5181,19 @@
       <c r="R77">
         <v>40</v>
       </c>
-    </row>
-    <row r="78" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S77" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="78" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="B78" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="C78" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="D78">
         <v>2</v>
@@ -5015,16 +5240,19 @@
       <c r="R78">
         <v>49</v>
       </c>
-    </row>
-    <row r="79" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S78" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="79" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="B79" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="C79" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D79">
         <v>4</v>
@@ -5071,16 +5299,19 @@
       <c r="R79">
         <v>52</v>
       </c>
-    </row>
-    <row r="80" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S79" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="80" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="B80" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="C80" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="D80">
         <v>3</v>
@@ -5127,16 +5358,19 @@
       <c r="R80">
         <v>38</v>
       </c>
-    </row>
-    <row r="81" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S80" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="81" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="B81" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C81" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="D81">
         <v>5</v>
@@ -5183,16 +5417,19 @@
       <c r="R81">
         <v>47</v>
       </c>
-    </row>
-    <row r="82" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S81" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="82" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="B82" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C82" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="D82">
         <v>1</v>
@@ -5239,16 +5476,19 @@
       <c r="R82">
         <v>41</v>
       </c>
-    </row>
-    <row r="83" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S82" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="83" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="B83" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="C83" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="D83">
         <v>1</v>
@@ -5295,16 +5535,19 @@
       <c r="R83">
         <v>42</v>
       </c>
-    </row>
-    <row r="84" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S83" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="84" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="B84" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="C84" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="D84">
         <v>1</v>
@@ -5351,16 +5594,19 @@
       <c r="R84">
         <v>39</v>
       </c>
-    </row>
-    <row r="85" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S84" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="85" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="B85" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="C85" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="D85">
         <v>2</v>
@@ -5407,16 +5653,19 @@
       <c r="R85">
         <v>39</v>
       </c>
-    </row>
-    <row r="86" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S85" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="86" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="B86" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="C86" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="D86">
         <v>1</v>
@@ -5463,16 +5712,19 @@
       <c r="R86">
         <v>44</v>
       </c>
-    </row>
-    <row r="87" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S86" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="87" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="B87" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="C87" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="D87">
         <v>2</v>
@@ -5519,16 +5771,19 @@
       <c r="R87">
         <v>53</v>
       </c>
-    </row>
-    <row r="88" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S87" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="88" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="B88" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="C88" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="D88">
         <v>2</v>
@@ -5575,16 +5830,19 @@
       <c r="R88">
         <v>51</v>
       </c>
-    </row>
-    <row r="89" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S88" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="89" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="B89" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C89" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="D89">
         <v>1</v>
@@ -5631,16 +5889,19 @@
       <c r="R89">
         <v>44</v>
       </c>
-    </row>
-    <row r="90" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S89" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="90" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="B90" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="C90" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D90">
         <v>1</v>
@@ -5687,16 +5948,19 @@
       <c r="R90">
         <v>59</v>
       </c>
-    </row>
-    <row r="91" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S90" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="91" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="B91" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="C91" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D91">
         <v>3</v>
@@ -5743,16 +6007,19 @@
       <c r="R91">
         <v>50</v>
       </c>
-    </row>
-    <row r="92" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S91" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="92" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="B92" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="C92" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="D92">
         <v>1</v>
@@ -5799,16 +6066,19 @@
       <c r="R92">
         <v>46</v>
       </c>
-    </row>
-    <row r="93" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S92" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="93" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="B93" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="C93" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="D93">
         <v>3</v>
@@ -5855,16 +6125,19 @@
       <c r="R93">
         <v>64</v>
       </c>
-    </row>
-    <row r="94" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S93" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="94" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="B94" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C94" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="D94">
         <v>1</v>
@@ -5911,16 +6184,19 @@
       <c r="R94">
         <v>38</v>
       </c>
-    </row>
-    <row r="95" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S94" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="95" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="B95" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="C95" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="D95">
         <v>1</v>
@@ -5961,22 +6237,25 @@
       <c r="P95">
         <v>1</v>
       </c>
-      <c r="Q95" t="s">
-        <v>75</v>
-      </c>
-      <c r="R95" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="96" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="Q95">
+        <v>43</v>
+      </c>
+      <c r="R95">
+        <v>57</v>
+      </c>
+      <c r="S95" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="96" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="B96" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C96" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="D96">
         <v>1</v>
@@ -5988,51 +6267,54 @@
         <v>1378266</v>
       </c>
       <c r="G96">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="H96">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="I96">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J96">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="K96">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L96">
         <v>0</v>
       </c>
       <c r="M96">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N96">
         <v>0</v>
       </c>
       <c r="O96">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P96">
         <v>2</v>
       </c>
-      <c r="Q96" t="s">
-        <v>78</v>
-      </c>
-      <c r="R96" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="97" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="Q96">
+        <v>49</v>
+      </c>
+      <c r="R96">
+        <v>51</v>
+      </c>
+      <c r="S96" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="97" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="B97" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C97" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="D97">
         <v>7</v>
@@ -6044,16 +6326,16 @@
         <v>1378267</v>
       </c>
       <c r="G97">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H97">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I97">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J97">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="K97">
         <v>0</v>
@@ -6062,33 +6344,36 @@
         <v>0</v>
       </c>
       <c r="M97">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="N97">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O97">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="P97">
-        <v>2</v>
-      </c>
-      <c r="Q97" t="s">
-        <v>78</v>
-      </c>
-      <c r="R97" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="98" spans="1:18" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+      <c r="Q97">
+        <v>53</v>
+      </c>
+      <c r="R97">
+        <v>47</v>
+      </c>
+      <c r="S97" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="98" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="B98" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="C98" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="D98">
         <v>5</v>
@@ -6100,51 +6385,54 @@
         <v>1378268</v>
       </c>
       <c r="G98">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="H98">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="I98">
         <v>0</v>
       </c>
       <c r="J98">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K98">
         <v>0</v>
       </c>
       <c r="L98">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M98">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="N98">
         <v>0</v>
       </c>
       <c r="O98">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="P98">
         <v>1</v>
       </c>
-      <c r="Q98" t="s">
-        <v>78</v>
-      </c>
-      <c r="R98" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="99" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="Q98">
+        <v>53</v>
+      </c>
+      <c r="R98">
+        <v>47</v>
+      </c>
+      <c r="S98" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="99" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="B99" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="C99" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="D99">
         <v>4</v>
@@ -6156,51 +6444,54 @@
         <v>1378269</v>
       </c>
       <c r="G99">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="H99">
         <v>0</v>
       </c>
       <c r="I99">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="J99">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="K99">
         <v>0</v>
       </c>
       <c r="L99">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M99">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N99">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O99">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="P99">
-        <v>2</v>
-      </c>
-      <c r="Q99" t="s">
-        <v>78</v>
-      </c>
-      <c r="R99" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="100" spans="1:18" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+      <c r="Q99">
+        <v>64</v>
+      </c>
+      <c r="R99">
+        <v>36</v>
+      </c>
+      <c r="S99" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="100" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B100" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="C100" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="D100">
         <v>2</v>
@@ -6215,48 +6506,51 @@
         <v>0</v>
       </c>
       <c r="H100">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="I100">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="J100">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="K100">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="L100">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M100">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N100">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="O100">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="P100">
-        <v>2</v>
-      </c>
-      <c r="Q100" t="s">
-        <v>78</v>
-      </c>
-      <c r="R100" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="101" spans="1:18" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+      <c r="Q100">
+        <v>48</v>
+      </c>
+      <c r="R100">
+        <v>52</v>
+      </c>
+      <c r="S100" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="101" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B101" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="C101" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="D101">
         <v>4</v>
@@ -6268,40 +6562,102 @@
         <v>1378271</v>
       </c>
       <c r="G101">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="H101">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I101">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J101">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="K101">
         <v>0</v>
       </c>
       <c r="L101">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="M101">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="N101">
         <v>0</v>
       </c>
       <c r="O101">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="P101">
         <v>0</v>
       </c>
-      <c r="Q101" t="s">
-        <v>78</v>
-      </c>
-      <c r="R101" t="s">
-        <v>78</v>
+      <c r="Q101">
+        <v>68</v>
+      </c>
+      <c r="R101">
+        <v>32</v>
+      </c>
+      <c r="S101" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="102" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A102" s="2">
+        <v>45845</v>
+      </c>
+      <c r="B102" t="s">
+        <v>31</v>
+      </c>
+      <c r="C102" t="s">
+        <v>21</v>
+      </c>
+      <c r="D102">
+        <v>1</v>
+      </c>
+      <c r="E102">
+        <v>1</v>
+      </c>
+      <c r="F102">
+        <v>1378272</v>
+      </c>
+      <c r="G102">
+        <v>7</v>
+      </c>
+      <c r="H102">
+        <v>4</v>
+      </c>
+      <c r="I102">
+        <v>1</v>
+      </c>
+      <c r="J102">
+        <v>1</v>
+      </c>
+      <c r="K102">
+        <v>0</v>
+      </c>
+      <c r="L102">
+        <v>0</v>
+      </c>
+      <c r="M102">
+        <v>1</v>
+      </c>
+      <c r="N102">
+        <v>1</v>
+      </c>
+      <c r="O102">
+        <v>0</v>
+      </c>
+      <c r="P102">
+        <v>0</v>
+      </c>
+      <c r="Q102">
+        <v>57</v>
+      </c>
+      <c r="R102">
+        <v>43</v>
+      </c>
+      <c r="S102" t="s">
+        <v>41</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
🔁 Integración completa con Flow: confirmación, código generado y mostrado
</commit_message>
<xml_diff>
--- a/Ligas/Liga_bolivia_2025.xlsx
+++ b/Ligas/Liga_bolivia_2025.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\raque\Desktop\ligas_datas\rockongo_web\Ligas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48404140-E6B9-4FB2-BD04-E31E62413E54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E341AFD-50BC-4CF0-B06A-03B0DB594903}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -269,6 +269,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
+  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -323,7 +326,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -628,18 +631,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:S102"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B79" workbookViewId="0">
-      <selection activeCell="C104" sqref="C104"/>
+    <sheetView tabSelected="1" topLeftCell="A85" workbookViewId="0">
+      <selection activeCell="G109" sqref="G109"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="20.88671875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.5546875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="12.77734375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="13" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="12.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Agrego nueva liga a RockData
</commit_message>
<xml_diff>
--- a/Ligas/Liga_bolivia_2025.xlsx
+++ b/Ligas/Liga_bolivia_2025.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\raque\Desktop\ligas_datas\rockongo_web\Ligas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94416F9E-A8C4-4082-AF78-EBDB0F2A1EEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39B4C70A-59D6-4B6E-93D5-2983D12EE41F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="478" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="486" uniqueCount="91">
   <si>
     <t>Fecha</t>
   </si>
@@ -287,6 +287,12 @@
   </si>
   <si>
     <t>2025-07-22</t>
+  </si>
+  <si>
+    <t>2025-07-29</t>
+  </si>
+  <si>
+    <t>2025-07-30</t>
   </si>
 </sst>
 </file>
@@ -294,7 +300,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="167" formatCode="yyyy/mm/dd;@"/>
+    <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -350,9 +356,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -655,16 +659,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:S116"/>
+  <dimension ref="A1:S118"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A100" workbookViewId="0">
-      <selection activeCell="G117" sqref="G117"/>
+    <sheetView tabSelected="1" topLeftCell="A109" workbookViewId="0">
+      <selection activeCell="G118" sqref="G118"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="18" bestFit="1" customWidth="1"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
@@ -7508,6 +7509,124 @@
       </c>
       <c r="S116" t="s">
         <v>25</v>
+      </c>
+    </row>
+    <row r="117" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A117" t="s">
+        <v>89</v>
+      </c>
+      <c r="B117" t="s">
+        <v>29</v>
+      </c>
+      <c r="C117" t="s">
+        <v>32</v>
+      </c>
+      <c r="D117">
+        <v>1</v>
+      </c>
+      <c r="E117">
+        <v>2</v>
+      </c>
+      <c r="F117">
+        <v>1378247</v>
+      </c>
+      <c r="G117">
+        <v>3</v>
+      </c>
+      <c r="H117">
+        <v>1</v>
+      </c>
+      <c r="I117">
+        <v>0</v>
+      </c>
+      <c r="J117">
+        <v>2</v>
+      </c>
+      <c r="K117">
+        <v>0</v>
+      </c>
+      <c r="L117">
+        <v>1</v>
+      </c>
+      <c r="M117">
+        <v>0</v>
+      </c>
+      <c r="N117">
+        <v>2</v>
+      </c>
+      <c r="O117">
+        <v>1</v>
+      </c>
+      <c r="P117">
+        <v>0</v>
+      </c>
+      <c r="Q117">
+        <v>50</v>
+      </c>
+      <c r="R117">
+        <v>50</v>
+      </c>
+      <c r="S117" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="118" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A118" t="s">
+        <v>90</v>
+      </c>
+      <c r="B118" t="s">
+        <v>23</v>
+      </c>
+      <c r="C118" t="s">
+        <v>37</v>
+      </c>
+      <c r="D118">
+        <v>4</v>
+      </c>
+      <c r="E118">
+        <v>1</v>
+      </c>
+      <c r="F118">
+        <v>1370697</v>
+      </c>
+      <c r="G118">
+        <v>3</v>
+      </c>
+      <c r="H118">
+        <v>3</v>
+      </c>
+      <c r="I118">
+        <v>4</v>
+      </c>
+      <c r="J118">
+        <v>4</v>
+      </c>
+      <c r="K118">
+        <v>1</v>
+      </c>
+      <c r="L118">
+        <v>0</v>
+      </c>
+      <c r="M118">
+        <v>2</v>
+      </c>
+      <c r="N118">
+        <v>0</v>
+      </c>
+      <c r="O118">
+        <v>2</v>
+      </c>
+      <c r="P118">
+        <v>1</v>
+      </c>
+      <c r="Q118">
+        <v>42</v>
+      </c>
+      <c r="R118">
+        <v>58</v>
+      </c>
+      <c r="S118" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>